<commit_message>
03/05/2023 - Omar - Terminadas las pruebas de usabilidad
</commit_message>
<xml_diff>
--- a/usability_tests/Results.xlsx
+++ b/usability_tests/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
   <si>
     <t>ROUND 1</t>
   </si>
@@ -54,75 +54,12 @@
   <si>
     <t>USABILITY TESTS RESULTS FROM LOMAP-ES3A</t>
   </si>
-  <si>
-    <t>User 1</t>
-  </si>
-  <si>
-    <t>User 2</t>
-  </si>
-  <si>
-    <t>User 3</t>
-  </si>
-  <si>
-    <t>User 4</t>
-  </si>
-  <si>
-    <t>User 5</t>
-  </si>
-  <si>
-    <t>User 6</t>
-  </si>
-  <si>
-    <t>User 7</t>
-  </si>
-  <si>
-    <t>User 8</t>
-  </si>
-  <si>
-    <t>User 9</t>
-  </si>
-  <si>
-    <t>User 10</t>
-  </si>
-  <si>
-    <t>User 11</t>
-  </si>
-  <si>
-    <t>User 12</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Task Time</t>
-  </si>
-  <si>
-    <t>Task Completion</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>In case of Gender, we'll be using:</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,8 +90,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,14 +130,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -278,143 +217,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="13"/>
@@ -429,9 +236,6 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -441,29 +245,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,6 +496,18 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -831,6 +628,18 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -951,6 +760,18 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1229,6 +1050,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1243,12 +1073,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-164871248"/>
-        <c:axId val="-164870160"/>
+        <c:axId val="1325718080"/>
+        <c:axId val="1325725152"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-164871248"/>
+        <c:axId val="1325718080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1285,7 +1115,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-164870160"/>
+        <c:crossAx val="1325725152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1293,7 +1123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-164870160"/>
+        <c:axId val="1325725152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1343,7 +1173,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-164871248"/>
+        <c:crossAx val="1325718080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1582,6 +1412,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1596,12 +1435,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-166746608"/>
-        <c:axId val="-166752592"/>
+        <c:axId val="1325727872"/>
+        <c:axId val="1325720800"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-166746608"/>
+        <c:axId val="1325727872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1638,7 +1477,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166752592"/>
+        <c:crossAx val="1325720800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1646,7 +1485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-166752592"/>
+        <c:axId val="1325720800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,7 +1535,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-166746608"/>
+        <c:crossAx val="1325727872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1935,6 +1774,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1949,12 +1797,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-78687664"/>
-        <c:axId val="-78695280"/>
+        <c:axId val="1325728960"/>
+        <c:axId val="1325730048"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-78687664"/>
+        <c:axId val="1325728960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,7 +1839,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-78695280"/>
+        <c:crossAx val="1325730048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1999,7 +1847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-78695280"/>
+        <c:axId val="1325730048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,7 +1897,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-78687664"/>
+        <c:crossAx val="1325728960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2364,6 +2212,18 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2487,6 +2347,18 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2610,6 +2482,18 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2936,6 +2820,18 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3211,6 +3107,12 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3493,6 +3395,12 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3775,6 +3683,12 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4054,6 +3968,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>186.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>169.09</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4068,12 +3991,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-164869616"/>
-        <c:axId val="-164869072"/>
+        <c:axId val="1325722976"/>
+        <c:axId val="1325724608"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-164869616"/>
+        <c:axId val="1325722976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4110,7 +4033,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-164869072"/>
+        <c:crossAx val="1325724608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4118,7 +4041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-164869072"/>
+        <c:axId val="1325724608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4168,7 +4091,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-164869616"/>
+        <c:crossAx val="1325722976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4410,6 +4333,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>162.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>142.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160.41</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4424,12 +4356,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-164874512"/>
-        <c:axId val="-164873424"/>
+        <c:axId val="1325722432"/>
+        <c:axId val="1325720256"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-164874512"/>
+        <c:axId val="1325722432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4466,7 +4398,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-164873424"/>
+        <c:crossAx val="1325720256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4474,7 +4406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-164873424"/>
+        <c:axId val="1325720256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4524,7 +4456,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-164874512"/>
+        <c:crossAx val="1325722432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4766,6 +4698,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>147.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>155.58000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4780,12 +4721,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-164873968"/>
-        <c:axId val="-164872336"/>
+        <c:axId val="1325723520"/>
+        <c:axId val="1325719712"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-164873968"/>
+        <c:axId val="1325723520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4822,7 +4763,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-164872336"/>
+        <c:crossAx val="1325719712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4830,7 +4771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-164872336"/>
+        <c:axId val="1325719712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4880,7 +4821,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-164873968"/>
+        <c:crossAx val="1325723520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12159,444 +12100,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AA18"/>
+  <dimension ref="B1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="2:17" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
-    <row r="2" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:27" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="13" t="s">
+    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="15"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="14"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="U3" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="V3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="W3" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="8">
+        <v>0.25</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="8">
+        <v>0.5</v>
+      </c>
       <c r="I4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="7"/>
+      <c r="J4" s="7">
+        <v>186.89</v>
+      </c>
       <c r="L4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="7"/>
-      <c r="S4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="T4" s="20"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="19"/>
-      <c r="Z4">
-        <v>1</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>32</v>
+      <c r="M4" s="7">
+        <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="9">
+        <v>0.25</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="9">
+        <v>0.5</v>
+      </c>
       <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="3">
+        <v>138.44</v>
+      </c>
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="3"/>
-      <c r="S5" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="T5" s="21"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="17"/>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>33</v>
+      <c r="M5" s="3">
+        <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="9">
+        <v>0.25</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="3">
+        <v>169.09</v>
+      </c>
       <c r="L6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="S6" s="25" t="s">
-        <v>15</v>
+      <c r="M6" s="3">
+        <v>100</v>
       </c>
-      <c r="T6" s="21"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="17"/>
     </row>
-    <row r="7" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="S7" s="34" t="s">
-        <v>16</v>
+      <c r="D7" s="10">
+        <v>0.25</v>
       </c>
-      <c r="T7" s="28"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="30"/>
     </row>
-    <row r="8" spans="2:27" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="2:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="14"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="T8" s="33" t="e">
-        <f>AVERAGE(T4:T7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U8" s="33" t="e">
-        <f t="shared" ref="U8:W8" si="0">AVERAGE(U4:U7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V8" s="33" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W8" s="33" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>0.5</v>
+      </c>
       <c r="F9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8">
+        <v>0.75</v>
+      </c>
       <c r="I9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="7"/>
+      <c r="J9" s="7">
+        <v>162.03</v>
+      </c>
       <c r="L9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="7"/>
-      <c r="S9" s="31" t="s">
-        <v>17</v>
+      <c r="M9" s="7">
+        <v>100</v>
       </c>
-      <c r="T9" s="20"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="19"/>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9">
+        <v>0.25</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="G10" s="9">
+        <v>0.25</v>
+      </c>
       <c r="I10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3">
+        <v>142.80000000000001</v>
+      </c>
       <c r="L10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="3"/>
-      <c r="S10" s="26" t="s">
-        <v>18</v>
+      <c r="M10" s="3">
+        <v>100</v>
       </c>
-      <c r="T10" s="21"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="17"/>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="9">
+        <v>0.25</v>
+      </c>
       <c r="I11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3">
+        <v>160.41</v>
+      </c>
       <c r="L11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="3"/>
-      <c r="S11" s="26" t="s">
-        <v>19</v>
+      <c r="M11" s="3">
+        <v>100</v>
       </c>
-      <c r="T11" s="21"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="17"/>
     </row>
-    <row r="12" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="S12" s="27" t="s">
-        <v>20</v>
+      <c r="D12" s="10">
+        <v>0</v>
       </c>
-      <c r="T12" s="28"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="30"/>
     </row>
-    <row r="13" spans="2:27" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="2:17" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="14"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="T13" s="33" t="e">
-        <f>AVERAGE(T9:T12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U13" s="33" t="e">
-        <f t="shared" ref="U13" si="1">AVERAGE(U9:U12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V13" s="33" t="e">
-        <f t="shared" ref="V13" si="2">AVERAGE(V9:V12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W13" s="33" t="e">
-        <f t="shared" ref="W13" si="3">AVERAGE(W9:W12)</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8">
+        <v>0.25</v>
+      </c>
       <c r="F14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="8"/>
+      <c r="G14" s="8">
+        <v>0.75</v>
+      </c>
       <c r="I14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="7"/>
+      <c r="J14" s="7">
+        <v>147.4</v>
+      </c>
       <c r="L14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="7"/>
-      <c r="S14" s="31" t="s">
-        <v>21</v>
+      <c r="M14" s="7">
+        <v>100</v>
       </c>
-      <c r="T14" s="20"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="19"/>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9">
+        <v>0.5</v>
+      </c>
       <c r="F15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9">
+        <v>0.25</v>
+      </c>
       <c r="I15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="3"/>
+      <c r="J15" s="3">
+        <v>134.80000000000001</v>
+      </c>
       <c r="L15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="3"/>
-      <c r="S15" s="26" t="s">
-        <v>22</v>
+      <c r="M15" s="3">
+        <v>100</v>
       </c>
-      <c r="T15" s="21"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="17"/>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="9">
+        <v>0.25</v>
+      </c>
       <c r="I16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="3"/>
+      <c r="J16" s="3">
+        <v>155.58000000000001</v>
+      </c>
       <c r="L16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M16" s="3"/>
+      <c r="M16" s="3">
+        <v>100</v>
+      </c>
       <c r="P16" s="11"/>
-      <c r="S16" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="T16" s="21"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="17"/>
     </row>
-    <row r="17" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="S17" s="27" t="s">
-        <v>24</v>
+      <c r="D17" s="9">
+        <v>0</v>
       </c>
-      <c r="T17" s="28"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="29"/>
-      <c r="W17" s="30"/>
     </row>
-    <row r="18" spans="3:23" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S18" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="T18" s="33" t="e">
-        <f>AVERAGE(T14:T17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U18" s="33" t="e">
-        <f t="shared" ref="U18" si="4">AVERAGE(U14:U17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V18" s="33" t="e">
-        <f t="shared" ref="V18" si="5">AVERAGE(V14:V17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W18" s="33" t="e">
-        <f t="shared" ref="W18" si="6">AVERAGE(W14:W17)</f>
-        <v>#DIV/0!</v>
-      </c>
+    <row r="18" spans="3:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>